<commit_message>
Corrección año de reporte ventas
</commit_message>
<xml_diff>
--- a/Nana&Rene/PedidosTest.xlsx
+++ b/Nana&Rene/PedidosTest.xlsx
@@ -47,7 +47,7 @@
     <t>ID</t>
   </si>
   <si>
-    <t>1-Torta,2-Queque,</t>
+    <t>2-Queque,1-Torta,</t>
   </si>
   <si>
     <t>05-10-2019</t>
@@ -65,7 +65,7 @@
     <t>9-48485930</t>
   </si>
   <si>
-    <t>Retirado</t>
+    <t>Pendiente</t>
   </si>
   <si>
     <t>1-Kuchen Manzana,</t>
@@ -155,6 +155,9 @@
     <t>9-75819247</t>
   </si>
   <si>
+    <t>Finalizado</t>
+  </si>
+  <si>
     <t>16-10-2019</t>
   </si>
   <si>
@@ -168,9 +171,6 @@
   </si>
   <si>
     <t>2-Torta,</t>
-  </si>
-  <si>
-    <t>20-11-2019</t>
   </si>
   <si>
     <t>albertitohurtado@gmail.com</t>
@@ -454,7 +454,7 @@
         <v>46</v>
       </c>
       <c r="G7" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="H7" t="n">
         <v>1020.0</v>
@@ -477,19 +477,19 @@
         <v>43</v>
       </c>
       <c r="C8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" t="s">
         <v>47</v>
-      </c>
-      <c r="D8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8" t="s">
-        <v>50</v>
-      </c>
-      <c r="G8" t="s">
-        <v>17</v>
       </c>
       <c r="H8" t="n">
         <v>450.0</v>
@@ -506,13 +506,13 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
         <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
         <v>14</v>
@@ -524,7 +524,7 @@
         <v>16</v>
       </c>
       <c r="G9" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="H9" t="n">
         <v>10000.0</v>

</xml_diff>